<commit_message>
Updated with initial Previs tool
Unlike google docs, we can put letters near the dots.
</commit_message>
<xml_diff>
--- a/patternSystems/Supreme System Blue Book/System Equations.xlsx
+++ b/patternSystems/Supreme System Blue Book/System Equations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\Documents\Programming Projects\InterpolationDraping\InterpolationDraping\Supreme System Blue Book\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\Documents\Programming Projects\InterpolationDraping\InterpolationDraping\patternSystems\Supreme System Blue Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94430F26-B8FF-4D5C-A47F-BD3BD7D20949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4D2C93-E3DA-47FE-A41B-8CE8273912BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="229">
   <si>
     <t>Document Source: Link</t>
   </si>
@@ -837,7 +837,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -846,7 +846,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1046,15 +1052,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -1074,13 +1078,18 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1099,20 +1108,1975 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Previsualization v0</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2F30A523-E106-4DFE-8911-58EA24BFB1FB}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{8FA6837A-BE49-4B14-AFC5-57AC3AACD106}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{9AD04BE3-1739-4672-8A90-A937676C5230}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2EB09C2E-AE5E-4A6B-8B42-6B8D8D373FC7}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{9F3721B5-3F6B-44FC-9C9F-8D15FDCB05B0}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{27E65130-BFCA-4F6B-98C9-9ABABB6D078A}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{C327C17D-FD5F-4474-B865-2FAE79B49D00}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{888CD470-1D77-4FC3-87D6-39AE4B0A7605}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{3AFBCF27-5601-42F9-9DD8-2F310330D91C}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{D2C0198B-3352-44C8-BEE0-D4490275ACC1}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{0FC7851A-4D93-4F42-8002-A89D93571E58}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{9D057B48-572B-482C-967E-64FFD6086530}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{E44089BC-71FD-48C6-BFEA-A85F7AA47D78}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{4588286C-D618-4592-8B62-BACE864430F2}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{E69FC904-40E9-48AA-AECC-4F8B705C3F13}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{6C0B4986-7426-4E1E-9F1F-F501FF714E09}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{1BB52CEE-618B-43D4-887F-D5E9510781B2}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{D5A9C904-FA6E-48F4-9818-1FD853056F97}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000012-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{ACFE764A-FF62-48E7-848A-C410D1F19329}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000013-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{1A039FD2-4284-41C8-9934-3F9CBEDBAB71}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000014-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{49F26B7E-34A1-4E59-8A7E-36D4D6A63330}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000015-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{C3D739D9-9D16-40CA-8364-EE8C1CAD4346}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000016-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="22"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{22350D81-6280-4F8F-BE17-4AD3895DB61B}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000017-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="23"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{216CCA6F-1A91-448A-99D3-1ECBE24B434A}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000018-8901-42DA-B725-A71E71B7917A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Coat Equations'!$O$45:$O$68</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-5.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-6.833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-11.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-11.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-11.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-14.166666666666666</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-18.25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-18.25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-14.166666666666666</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-16.833333333333332</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-2.6666666666666665</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-2.6666666666666665</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-6.833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-11.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-17.280254650490317</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Coat Equations'!$P$45:$P$68</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-8.3333333333333321</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-24.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-8.3333333333333321</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-8.3333333333333321</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-8.3333333333333321</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-8.3333333333333321</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-24.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-8.3333333333333321</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-8.3333333333333321</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-8.3333333333333321</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-3.291062801932366</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-3.291062801932366</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.76454783761855882</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-2.5397977258648643</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>'Coat Equations'!$N$45:$N$68</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="24"/>
+                  <c:pt idx="0">
+                    <c:v>A</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>V</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>B</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>C</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>D</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>E</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>F</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>H</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>S</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>G</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>L</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>U</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>W</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>N</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>I</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>O</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>X</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Q</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>T</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>R</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>K</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>Z</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>J</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>P</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8901-42DA-B725-A71E71B7917A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="903581104"/>
+        <c:axId val="903582544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="903581104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="903582544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="903582544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="903581104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>178250</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>32084</xdr:rowOff>
+      <xdr:colOff>81996</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>48127</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>207445</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>131750</xdr:rowOff>
+      <xdr:colOff>111191</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>147792</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1141,7 +3105,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8544208" y="6120063"/>
+          <a:off x="8447954" y="7243011"/>
           <a:ext cx="4296395" cy="5634192"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1149,6 +3113,42 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>320844</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>132347</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>16044</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>104274</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{514184CD-AB48-52D7-DEB5-0F290A47D3B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1432,8 +3432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F83"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1486,56 +3486,56 @@
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
     </row>
     <row r="15" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
@@ -1548,10 +3548,10 @@
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="9" t="s">
         <v>151</v>
       </c>
       <c r="E23" t="s">
@@ -1559,77 +3559,77 @@
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="24">
         <v>45</v>
       </c>
       <c r="E24" t="s">
         <v>153</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="28">
         <v>25</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="25">
         <v>23</v>
       </c>
       <c r="E25" t="s">
         <v>154</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="23">
         <f>ROUNDDOWN(F24/2.54*8,0)/8</f>
         <v>9.75</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="25">
         <v>38</v>
       </c>
       <c r="E26" t="s">
         <v>155</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="23">
         <f>ROUNDUP(F24/2.54*8,0)/8</f>
         <v>9.875</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="25">
         <v>32</v>
       </c>
       <c r="E27" t="s">
         <v>201</v>
       </c>
-      <c r="F27" cm="1">
+      <c r="F27" s="23" cm="1">
         <f t="array" ref="F27">ROUNDEIGHTH((F24/2.54))</f>
         <v>9.875</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="25">
         <v>37</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="7"/>
+      <c r="C29" s="25"/>
       <c r="E29" t="s">
         <v>162</v>
       </c>
@@ -1638,10 +3638,10 @@
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="25">
         <v>70</v>
       </c>
       <c r="E30">
@@ -1652,13 +3652,13 @@
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="26">
         <v>43</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="18" t="s">
         <v>214</v>
       </c>
       <c r="F31">
@@ -1666,7 +3666,7 @@
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E32" s="20" t="s">
+      <c r="E32" s="18" t="s">
         <v>156</v>
       </c>
       <c r="F32">
@@ -1674,13 +3674,13 @@
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E33" s="18" t="s">
         <v>215</v>
       </c>
       <c r="F33">
@@ -1688,11 +3688,11 @@
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="7"/>
-      <c r="E34" s="20" t="s">
+      <c r="C34" s="25"/>
+      <c r="E34" s="18" t="s">
         <v>157</v>
       </c>
       <c r="F34">
@@ -1700,11 +3700,11 @@
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="E35" s="20" t="s">
+      <c r="C35" s="25"/>
+      <c r="E35" s="18" t="s">
         <v>216</v>
       </c>
       <c r="F35">
@@ -1712,11 +3712,11 @@
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="E36" s="20" t="s">
+      <c r="C36" s="25"/>
+      <c r="E36" s="18" t="s">
         <v>158</v>
       </c>
       <c r="F36">
@@ -1724,11 +3724,11 @@
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="E37" s="20" t="s">
+      <c r="C37" s="25"/>
+      <c r="E37" s="18" t="s">
         <v>217</v>
       </c>
       <c r="F37">
@@ -1736,11 +3736,11 @@
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="E38" s="20" t="s">
+      <c r="C38" s="25"/>
+      <c r="E38" s="18" t="s">
         <v>159</v>
       </c>
       <c r="F38">
@@ -1748,11 +3748,11 @@
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="E39" s="20" t="s">
+      <c r="C39" s="25"/>
+      <c r="E39" s="18" t="s">
         <v>218</v>
       </c>
       <c r="F39">
@@ -1760,11 +3760,11 @@
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="E40" s="20" t="s">
+      <c r="C40" s="25"/>
+      <c r="E40" s="18" t="s">
         <v>160</v>
       </c>
       <c r="F40">
@@ -1772,11 +3772,11 @@
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="7"/>
-      <c r="E41" s="20" t="s">
+      <c r="C41" s="25"/>
+      <c r="E41" s="18" t="s">
         <v>219</v>
       </c>
       <c r="F41">
@@ -1784,11 +3784,11 @@
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="9"/>
-      <c r="E42" s="20" t="s">
+      <c r="C42" s="26"/>
+      <c r="E42" s="18" t="s">
         <v>163</v>
       </c>
       <c r="F42">
@@ -1796,7 +3796,7 @@
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E43" s="20" t="s">
+      <c r="E43" s="18" t="s">
         <v>220</v>
       </c>
       <c r="F43">
@@ -1807,8 +3807,8 @@
       <c r="B44" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C44" s="5"/>
-      <c r="E44" s="20" t="s">
+      <c r="C44" s="24"/>
+      <c r="E44" s="18" t="s">
         <v>164</v>
       </c>
       <c r="F44">
@@ -1816,14 +3816,14 @@
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="7"/>
+      <c r="C45" s="25"/>
       <c r="D45" t="s">
         <v>30</v>
       </c>
-      <c r="E45" s="20" t="s">
+      <c r="E45" s="18" t="s">
         <v>221</v>
       </c>
       <c r="F45">
@@ -1831,54 +3831,54 @@
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="7"/>
+      <c r="C46" s="25"/>
       <c r="D46" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="7"/>
+      <c r="C47" s="25"/>
       <c r="D47" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C48" s="7"/>
+      <c r="C48" s="25"/>
       <c r="D48" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C49" s="9"/>
+      <c r="C49" s="26"/>
       <c r="D49" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="9" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C52" s="14"/>
+      <c r="C52" s="27"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
@@ -1989,13 +3989,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="15" t="s">
         <v>126</v>
       </c>
       <c r="E2" t="s">
@@ -2012,13 +4012,13 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="7" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2733,10 +4733,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BBB0D73-498E-414D-A33D-744DBB5FBF62}">
-  <dimension ref="A2:R69"/>
+  <dimension ref="A2:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView topLeftCell="A19" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2858,12 +4858,12 @@
         <v>228</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>199</v>
       </c>
@@ -2874,7 +4874,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>200</v>
       </c>
@@ -2894,62 +4894,66 @@
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B26" s="24" t="str">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B26" s="21" t="str">
         <f>_xlfn.CONCAT("From origin point A, square down just more than ",M50,"in. Mark these points along the line, measured from A:" )</f>
         <v>From origin point A, square down just more than 30in. Mark these points along the line, measured from A:</v>
       </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
       <c r="K26" t="s">
         <v>195</v>
       </c>
-      <c r="L26" s="21">
+      <c r="L26" s="19">
         <v>0</v>
       </c>
-      <c r="M26" s="21">
+      <c r="M26" s="19">
         <v>0</v>
       </c>
-      <c r="N26" s="21">
+      <c r="N26" s="19">
         <v>0</v>
       </c>
-      <c r="O26" s="21">
+      <c r="O26" s="19">
         <f>B9/2 -5</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
       <c r="K27" t="s">
         <v>196</v>
       </c>
-      <c r="L27" s="21">
+      <c r="L27" s="19">
         <v>0</v>
       </c>
-      <c r="M27" s="21">
+      <c r="M27" s="19">
         <v>0</v>
       </c>
-      <c r="N27" s="21">
+      <c r="N27" s="19">
         <f>((5*E5/6)+3.5)</f>
         <v>16.833333333333336</v>
       </c>
-      <c r="O27" s="21">
+      <c r="O27" s="19">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B28" t="str" cm="1">
         <f t="array" ref="B28">_xlfn.CONCAT("Point Z at ", ROUNDDOWN(M66,0), " &amp; ",MOD(ROUNDSIXTEENTH(M66),1)*16,"/16 in")</f>
         <v>Point Z at 3 &amp; 5/16 in</v>
@@ -2957,23 +4961,23 @@
       <c r="K28" t="s">
         <v>197</v>
       </c>
-      <c r="L28" s="21">
+      <c r="L28" s="19">
         <v>0</v>
       </c>
-      <c r="M28" s="21">
+      <c r="M28" s="19">
         <f>E5/3 +3</f>
         <v>8.3333333333333321</v>
       </c>
-      <c r="N28" s="21">
+      <c r="N28" s="19">
         <f>E5+2.25</f>
         <v>18.25</v>
       </c>
-      <c r="O28" s="21">
+      <c r="O28" s="19">
         <f>E5/3 +3</f>
         <v>8.3333333333333321</v>
       </c>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B29" t="str">
         <f>_xlfn.CONCAT("Point V at ", ROUNDEIGHTH(M46),"in")</f>
         <v>Point V at 5.375in</v>
@@ -2981,23 +4985,23 @@
       <c r="K29" t="s">
         <v>198</v>
       </c>
-      <c r="L29" s="21">
+      <c r="L29" s="19">
         <v>0</v>
       </c>
-      <c r="M29" s="21">
+      <c r="M29" s="19">
         <f>B9/4 +0.5</f>
         <v>18</v>
       </c>
-      <c r="N29" s="21">
+      <c r="N29" s="19">
         <f>E5+2.25</f>
         <v>18.25</v>
       </c>
-      <c r="O29" s="21">
+      <c r="O29" s="19">
         <f>B9/4 +0.5</f>
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B30" t="str">
         <f>_xlfn.CONCAT("Point B at ", ROUNDEIGHTH(M47),"in")</f>
         <v>Point B at 8.375in</v>
@@ -3005,23 +5009,23 @@
       <c r="K30" t="s">
         <v>202</v>
       </c>
-      <c r="L30" s="21">
+      <c r="L30" s="19">
         <v>0</v>
       </c>
-      <c r="M30" s="21">
+      <c r="M30" s="19">
         <f>M49</f>
         <v>24.333333333333332</v>
       </c>
-      <c r="N30" s="21">
+      <c r="N30" s="19">
         <f>L54</f>
         <v>11.5</v>
       </c>
-      <c r="O30" s="21">
+      <c r="O30" s="19">
         <f>M30</f>
         <v>24.333333333333332</v>
       </c>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
         <f>_xlfn.CONCAT("Point C at ", ROUNDEIGHTH(M48),"in")</f>
         <v>Point C at 18in</v>
@@ -3029,23 +5033,23 @@
       <c r="K31" t="s">
         <v>206</v>
       </c>
-      <c r="L31" s="21">
+      <c r="L31" s="19">
         <f>L54</f>
         <v>11.5</v>
       </c>
-      <c r="M31" s="21">
+      <c r="M31" s="19">
         <v>0</v>
       </c>
-      <c r="N31" s="21">
+      <c r="N31" s="19">
         <f>L31</f>
         <v>11.5</v>
       </c>
-      <c r="O31" s="21">
+      <c r="O31" s="19">
         <f>O30</f>
         <v>24.333333333333332</v>
       </c>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>_xlfn.CONCAT("Point D at ", ROUNDEIGHTH(M49),"in")</f>
         <v>Point D at 24.375in</v>
@@ -3053,18 +5057,18 @@
       <c r="K32" t="s">
         <v>207</v>
       </c>
-      <c r="L32" s="21">
+      <c r="L32" s="19">
         <f>L52</f>
         <v>6.833333333333333</v>
       </c>
-      <c r="M32" s="21">
+      <c r="M32" s="19">
         <v>0</v>
       </c>
-      <c r="N32" s="21">
+      <c r="N32" s="19">
         <f>L32</f>
         <v>6.833333333333333</v>
       </c>
-      <c r="O32" s="21">
+      <c r="O32" s="19">
         <f>O26</f>
         <v>30</v>
       </c>
@@ -3076,27 +5080,27 @@
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B34" s="24" t="str">
+      <c r="B34" s="21" t="str">
         <f>_xlfn.CONCAT("From origin point A, square across just more than ",ROUNDEIGHTH(L62),"in. Mark these points along the line, measured from A:")</f>
         <v>From origin point A, square across just more than 16.875in. Mark these points along the line, measured from A:</v>
       </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
@@ -3129,30 +5133,30 @@
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B41" s="25" t="s">
+      <c r="B41" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
       <c r="M41" cm="1">
         <f t="array" ref="M41">ROUNDDOWN(ROUNDSIXTEENTH(45),0)</f>
         <v>45</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="25"/>
-      <c r="I42" s="25"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
     </row>
     <row r="43" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
@@ -3177,6 +5181,15 @@
       <c r="M44" t="s">
         <v>4</v>
       </c>
+      <c r="N44" t="s">
+        <v>5</v>
+      </c>
+      <c r="O44" t="s">
+        <v>3</v>
+      </c>
+      <c r="P44" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B45" t="str">
@@ -3186,79 +5199,111 @@
       <c r="K45" t="s">
         <v>173</v>
       </c>
-      <c r="L45" s="21">
+      <c r="L45" s="19">
         <v>0</v>
       </c>
-      <c r="M45" s="21">
+      <c r="M45" s="19">
         <v>0</v>
       </c>
-      <c r="N45" s="21"/>
-      <c r="O45" s="21"/>
-      <c r="P45" s="21"/>
+      <c r="N45" t="s">
+        <v>173</v>
+      </c>
+      <c r="O45" s="19">
+        <f>-L45</f>
+        <v>0</v>
+      </c>
+      <c r="P45" s="19">
+        <f>-M45</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.3">
       <c r="K46" t="s">
         <v>175</v>
       </c>
-      <c r="L46" s="21">
+      <c r="L46" s="19">
         <v>0</v>
       </c>
-      <c r="M46" s="21">
+      <c r="M46" s="19">
         <f>E5/3</f>
         <v>5.333333333333333</v>
       </c>
-      <c r="N46" s="21"/>
-      <c r="O46" s="21"/>
-      <c r="P46" s="21"/>
+      <c r="N46" t="s">
+        <v>175</v>
+      </c>
+      <c r="O46" s="19">
+        <f t="shared" ref="O46:P68" si="0">-L46</f>
+        <v>0</v>
+      </c>
+      <c r="P46" s="19">
+        <f t="shared" si="0"/>
+        <v>-5.333333333333333</v>
+      </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B47" s="24" t="str">
+      <c r="B47" s="21" t="str">
         <f>_xlfn.CONCAT("From point B, square across just more than ",ROUNDEIGHTH(L59),"in. Mark these points along the line, measured from B:")</f>
         <v>From point B, square across just more than 18.25in. Mark these points along the line, measured from B:</v>
       </c>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
-      <c r="H47" s="24"/>
-      <c r="I47" s="24"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
       <c r="K47" t="s">
         <v>177</v>
       </c>
-      <c r="L47" s="21">
+      <c r="L47" s="19">
         <v>0</v>
       </c>
-      <c r="M47" s="21">
+      <c r="M47" s="19">
         <f>M46+3</f>
         <v>8.3333333333333321</v>
       </c>
-      <c r="N47" s="21"/>
-      <c r="O47" s="21"/>
-      <c r="P47" s="21"/>
+      <c r="N47" t="s">
+        <v>177</v>
+      </c>
+      <c r="O47" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P47" s="19">
+        <f t="shared" si="0"/>
+        <v>-8.3333333333333321</v>
+      </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
       <c r="K48" t="s">
         <v>178</v>
       </c>
-      <c r="L48" s="21">
+      <c r="L48" s="19">
         <v>0</v>
       </c>
-      <c r="M48" s="21">
+      <c r="M48" s="19">
         <f>B9/4 +0.5</f>
         <v>18</v>
       </c>
-      <c r="N48" s="21"/>
-      <c r="O48" s="21"/>
-      <c r="P48" s="21"/>
+      <c r="N48" t="s">
+        <v>178</v>
+      </c>
+      <c r="O48" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P48" s="19">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B49" t="str">
@@ -3268,16 +5313,24 @@
       <c r="K49" t="s">
         <v>179</v>
       </c>
-      <c r="L49" s="21">
+      <c r="L49" s="19">
         <v>0</v>
       </c>
-      <c r="M49" s="21">
+      <c r="M49" s="19">
         <f>B9/3 +1</f>
         <v>24.333333333333332</v>
       </c>
-      <c r="N49" s="21"/>
-      <c r="O49" s="21"/>
-      <c r="P49" s="21"/>
+      <c r="N49" t="s">
+        <v>179</v>
+      </c>
+      <c r="O49" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P49" s="19">
+        <f t="shared" si="0"/>
+        <v>-24.333333333333332</v>
+      </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B50" t="str">
@@ -3287,16 +5340,24 @@
       <c r="K50" t="s">
         <v>180</v>
       </c>
-      <c r="L50" s="21">
+      <c r="L50" s="19">
         <v>0</v>
       </c>
-      <c r="M50" s="21">
+      <c r="M50" s="19">
         <f>B9/2 -5</f>
         <v>30</v>
       </c>
-      <c r="N50" s="21"/>
-      <c r="O50" s="21"/>
-      <c r="P50" s="21"/>
+      <c r="N50" t="s">
+        <v>180</v>
+      </c>
+      <c r="O50" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P50" s="19">
+        <f t="shared" si="0"/>
+        <v>-30</v>
+      </c>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B51" t="str">
@@ -3306,17 +5367,25 @@
       <c r="K51" t="s">
         <v>181</v>
       </c>
-      <c r="L51" s="21">
+      <c r="L51" s="19">
         <f>E5/3</f>
         <v>5.333333333333333</v>
       </c>
-      <c r="M51" s="21">
+      <c r="M51" s="19">
         <f>M47</f>
         <v>8.3333333333333321</v>
       </c>
-      <c r="N51" s="21"/>
-      <c r="O51" s="21"/>
-      <c r="P51" s="21"/>
+      <c r="N51" t="s">
+        <v>181</v>
+      </c>
+      <c r="O51" s="19">
+        <f t="shared" si="0"/>
+        <v>-5.333333333333333</v>
+      </c>
+      <c r="P51" s="19">
+        <f t="shared" si="0"/>
+        <v>-8.3333333333333321</v>
+      </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B52" t="str">
@@ -3326,17 +5395,25 @@
       <c r="K52" t="s">
         <v>182</v>
       </c>
-      <c r="L52" s="21">
+      <c r="L52" s="19">
         <f>L51+1.5</f>
         <v>6.833333333333333</v>
       </c>
-      <c r="M52" s="21">
+      <c r="M52" s="19">
         <f>M47</f>
         <v>8.3333333333333321</v>
       </c>
-      <c r="N52" s="21"/>
-      <c r="O52" s="21"/>
-      <c r="P52" s="21"/>
+      <c r="N52" t="s">
+        <v>182</v>
+      </c>
+      <c r="O52" s="19">
+        <f t="shared" si="0"/>
+        <v>-6.833333333333333</v>
+      </c>
+      <c r="P52" s="19">
+        <f t="shared" si="0"/>
+        <v>-8.3333333333333321</v>
+      </c>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B53" t="str">
@@ -3346,84 +5423,116 @@
       <c r="K53" t="s">
         <v>183</v>
       </c>
-      <c r="L53" s="21">
+      <c r="L53" s="19">
         <f>E5/2</f>
         <v>8</v>
       </c>
-      <c r="M53" s="21">
+      <c r="M53" s="19">
         <f>M47</f>
         <v>8.3333333333333321</v>
       </c>
-      <c r="N53" s="21"/>
-      <c r="O53" s="21"/>
-      <c r="P53" s="21"/>
+      <c r="N53" t="s">
+        <v>183</v>
+      </c>
+      <c r="O53" s="19">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="P53" s="19">
+        <f t="shared" si="0"/>
+        <v>-8.3333333333333321</v>
+      </c>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.3">
       <c r="K54" t="s">
         <v>184</v>
       </c>
-      <c r="L54" s="21">
+      <c r="L54" s="19">
         <f>L53+3.5</f>
         <v>11.5</v>
       </c>
-      <c r="M54" s="21">
+      <c r="M54" s="19">
         <f>M47</f>
         <v>8.3333333333333321</v>
       </c>
-      <c r="N54" s="21"/>
-      <c r="O54" s="21"/>
-      <c r="P54" s="21"/>
+      <c r="N54" t="s">
+        <v>184</v>
+      </c>
+      <c r="O54" s="19">
+        <f t="shared" si="0"/>
+        <v>-11.5</v>
+      </c>
+      <c r="P54" s="19">
+        <f t="shared" si="0"/>
+        <v>-8.3333333333333321</v>
+      </c>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B55" s="24" t="str">
+      <c r="B55" s="21" t="str">
         <f>_xlfn.CONCAT("From point C, square across just more than ",ROUNDEIGHTH(L59),"in. Mark these points along the line, measured from C:")</f>
         <v>From point C, square across just more than 18.25in. Mark these points along the line, measured from C:</v>
       </c>
-      <c r="C55" s="24"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="24"/>
-      <c r="H55" s="24"/>
-      <c r="I55" s="24"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21"/>
+      <c r="I55" s="21"/>
       <c r="K55" t="s">
         <v>204</v>
       </c>
-      <c r="L55" s="21">
+      <c r="L55" s="19">
         <f>L54</f>
         <v>11.5</v>
       </c>
-      <c r="M55" s="21">
+      <c r="M55" s="19">
         <f>M48</f>
         <v>18</v>
       </c>
-      <c r="N55" s="21"/>
-      <c r="O55" s="21"/>
-      <c r="P55" s="21"/>
+      <c r="N55" t="s">
+        <v>204</v>
+      </c>
+      <c r="O55" s="19">
+        <f t="shared" si="0"/>
+        <v>-11.5</v>
+      </c>
+      <c r="P55" s="19">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="24"/>
-      <c r="G56" s="24"/>
-      <c r="H56" s="24"/>
-      <c r="I56" s="24"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
       <c r="K56" t="s">
         <v>205</v>
       </c>
-      <c r="L56" s="21">
+      <c r="L56" s="19">
         <f>L54</f>
         <v>11.5</v>
       </c>
-      <c r="M56" s="21">
+      <c r="M56" s="19">
         <f>M49</f>
         <v>24.333333333333332</v>
       </c>
-      <c r="N56" s="21"/>
-      <c r="O56" s="21"/>
-      <c r="P56" s="21"/>
+      <c r="N56" t="s">
+        <v>205</v>
+      </c>
+      <c r="O56" s="19">
+        <f t="shared" si="0"/>
+        <v>-11.5</v>
+      </c>
+      <c r="P56" s="19">
+        <f t="shared" si="0"/>
+        <v>-24.333333333333332</v>
+      </c>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B57" t="str">
@@ -3433,17 +5542,25 @@
       <c r="K57" t="s">
         <v>186</v>
       </c>
-      <c r="L57" s="21">
+      <c r="L57" s="19">
         <f>L54+(E5/6)</f>
         <v>14.166666666666666</v>
       </c>
-      <c r="M57" s="21">
+      <c r="M57" s="19">
         <f>M47</f>
         <v>8.3333333333333321</v>
       </c>
-      <c r="N57" s="21"/>
-      <c r="O57" s="21"/>
-      <c r="P57" s="21"/>
+      <c r="N57" t="s">
+        <v>186</v>
+      </c>
+      <c r="O57" s="19">
+        <f t="shared" si="0"/>
+        <v>-14.166666666666666</v>
+      </c>
+      <c r="P57" s="19">
+        <f t="shared" si="0"/>
+        <v>-8.3333333333333321</v>
+      </c>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B58" t="str">
@@ -3453,166 +5570,230 @@
       <c r="K58" t="s">
         <v>187</v>
       </c>
-      <c r="L58" s="21">
+      <c r="L58" s="19">
         <f>E5</f>
         <v>16</v>
       </c>
-      <c r="M58" s="21">
+      <c r="M58" s="19">
         <f>M47</f>
         <v>8.3333333333333321</v>
       </c>
-      <c r="N58" s="21"/>
-      <c r="O58" s="21"/>
-      <c r="P58" s="21"/>
+      <c r="N58" t="s">
+        <v>187</v>
+      </c>
+      <c r="O58" s="19">
+        <f t="shared" si="0"/>
+        <v>-16</v>
+      </c>
+      <c r="P58" s="19">
+        <f t="shared" si="0"/>
+        <v>-8.3333333333333321</v>
+      </c>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.3">
       <c r="K59" t="s">
         <v>188</v>
       </c>
-      <c r="L59" s="21">
+      <c r="L59" s="19">
         <f>L58+2.25</f>
         <v>18.25</v>
       </c>
-      <c r="M59" s="21">
+      <c r="M59" s="19">
         <f>M47</f>
         <v>8.3333333333333321</v>
       </c>
-      <c r="N59" s="21"/>
-      <c r="O59" s="21"/>
-      <c r="P59" s="21"/>
+      <c r="N59" t="s">
+        <v>188</v>
+      </c>
+      <c r="O59" s="19">
+        <f t="shared" si="0"/>
+        <v>-18.25</v>
+      </c>
+      <c r="P59" s="19">
+        <f t="shared" si="0"/>
+        <v>-8.3333333333333321</v>
+      </c>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B60" s="24" t="str">
+      <c r="B60" s="21" t="str">
         <f>_xlfn.CONCAT("From point D, square across just more than ",ROUNDEIGHTH(L56),"in. Mark point U at the intersection (",(ROUNDEIGHTH(L54)),"in away from line A).")</f>
         <v>From point D, square across just more than 11.5in. Mark point U at the intersection (11.5in away from line A).</v>
       </c>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="24"/>
-      <c r="H60" s="24"/>
-      <c r="I60" s="24"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="21"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="21"/>
       <c r="K60" t="s">
         <v>203</v>
       </c>
-      <c r="L60" s="21">
+      <c r="L60" s="19">
         <f>L59</f>
         <v>18.25</v>
       </c>
-      <c r="M60" s="21">
+      <c r="M60" s="19">
         <f>M48</f>
         <v>18</v>
       </c>
-      <c r="N60" s="21"/>
-      <c r="O60" s="21"/>
-      <c r="P60" s="21"/>
+      <c r="N60" t="s">
+        <v>203</v>
+      </c>
+      <c r="O60" s="19">
+        <f t="shared" si="0"/>
+        <v>-18.25</v>
+      </c>
+      <c r="P60" s="19">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B61" s="24"/>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="24"/>
-      <c r="F61" s="24"/>
-      <c r="G61" s="24"/>
-      <c r="H61" s="24"/>
-      <c r="I61" s="24"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
       <c r="K61" t="s">
         <v>208</v>
       </c>
-      <c r="L61" s="21">
+      <c r="L61" s="19">
         <f>L57</f>
         <v>14.166666666666666</v>
       </c>
-      <c r="M61" s="21">
+      <c r="M61" s="19">
         <f>M45</f>
         <v>0</v>
       </c>
-      <c r="N61" s="21"/>
-      <c r="O61" s="21"/>
-      <c r="P61" s="21"/>
+      <c r="N61" t="s">
+        <v>208</v>
+      </c>
+      <c r="O61" s="19">
+        <f t="shared" si="0"/>
+        <v>-14.166666666666666</v>
+      </c>
+      <c r="P61" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="2:16" x14ac:dyDescent="0.3">
       <c r="K62" t="s">
         <v>209</v>
       </c>
-      <c r="L62" s="21">
+      <c r="L62" s="19">
         <f>L61+(E5/6)</f>
         <v>16.833333333333332</v>
       </c>
-      <c r="M62" s="21">
+      <c r="M62" s="19">
         <f>M45</f>
         <v>0</v>
       </c>
-      <c r="N62" s="21"/>
-      <c r="O62" s="21"/>
-      <c r="P62" s="21"/>
+      <c r="N62" t="s">
+        <v>209</v>
+      </c>
+      <c r="O62" s="19">
+        <f t="shared" si="0"/>
+        <v>-16.833333333333332</v>
+      </c>
+      <c r="P62" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="24" t="str">
+      <c r="B63" s="21" t="str">
         <f>_xlfn.CONCAT("From point E, square down through O for a total length of around ", ((ROUNDDOWN(M50-M47,0)) + 3),"in down from I (inexact)")</f>
         <v>From point E, square down through O for a total length of around 24in down from I (inexact)</v>
       </c>
-      <c r="C63" s="24"/>
-      <c r="D63" s="24"/>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24"/>
-      <c r="G63" s="24"/>
-      <c r="H63" s="24"/>
-      <c r="I63" s="24"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="21"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="21"/>
       <c r="K63" t="s">
         <v>210</v>
       </c>
-      <c r="L63" s="21">
+      <c r="L63" s="19">
         <f>E5/6</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="M63" s="21">
+      <c r="M63" s="19">
         <f>M45</f>
         <v>0</v>
       </c>
-      <c r="N63" s="21"/>
-      <c r="O63" s="21"/>
-      <c r="P63" s="21"/>
+      <c r="N63" t="s">
+        <v>210</v>
+      </c>
+      <c r="O63" s="19">
+        <f t="shared" si="0"/>
+        <v>-2.6666666666666665</v>
+      </c>
+      <c r="P63" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B64" s="24"/>
-      <c r="C64" s="24"/>
-      <c r="D64" s="24"/>
-      <c r="E64" s="24"/>
-      <c r="F64" s="24"/>
-      <c r="G64" s="24"/>
-      <c r="H64" s="24"/>
-      <c r="I64" s="24"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="21"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
       <c r="K64" t="s">
         <v>211</v>
       </c>
-      <c r="L64" s="21">
+      <c r="L64" s="19">
         <f>L63</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="M64" s="21">
+      <c r="M64" s="19">
         <v>-0.75</v>
       </c>
-      <c r="N64" s="21"/>
-      <c r="O64" s="21"/>
-      <c r="P64" s="21"/>
+      <c r="N64" t="s">
+        <v>211</v>
+      </c>
+      <c r="O64" s="19">
+        <f t="shared" si="0"/>
+        <v>-2.6666666666666665</v>
+      </c>
+      <c r="P64" s="19">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
     </row>
     <row r="65" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K65" t="s">
         <v>212</v>
       </c>
-      <c r="L65" s="21">
+      <c r="L65" s="19">
         <f>L52</f>
         <v>6.833333333333333</v>
       </c>
-      <c r="M65" s="22">
+      <c r="M65" s="20">
         <f>(((L65-L64)/(L57-L64))*(M57-M64))</f>
         <v>3.291062801932366</v>
       </c>
-      <c r="N65" s="21"/>
-      <c r="O65" s="21"/>
-      <c r="P65" s="21"/>
+      <c r="N65" t="s">
+        <v>212</v>
+      </c>
+      <c r="O65" s="19">
+        <f t="shared" si="0"/>
+        <v>-6.833333333333333</v>
+      </c>
+      <c r="P65" s="19">
+        <f t="shared" si="0"/>
+        <v>-3.291062801932366</v>
+      </c>
     </row>
     <row r="66" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
@@ -3621,17 +5802,25 @@
       <c r="K66" t="s">
         <v>213</v>
       </c>
-      <c r="L66" s="21">
+      <c r="L66" s="19">
         <f>L45</f>
         <v>0</v>
       </c>
-      <c r="M66" s="21">
+      <c r="M66" s="19">
         <f>M65</f>
         <v>3.291062801932366</v>
       </c>
-      <c r="N66" s="21"/>
-      <c r="O66" s="21"/>
-      <c r="P66" s="21"/>
+      <c r="N66" t="s">
+        <v>213</v>
+      </c>
+      <c r="O66" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P66" s="19">
+        <f t="shared" si="0"/>
+        <v>-3.291062801932366</v>
+      </c>
     </row>
     <row r="67" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
@@ -3640,17 +5829,25 @@
       <c r="K67" t="s">
         <v>227</v>
       </c>
-      <c r="L67" s="21">
+      <c r="L67" s="19">
         <f>L54</f>
         <v>11.5</v>
       </c>
-      <c r="M67" s="22">
-        <f>(((L67-L66)/(L61-L66))*(M66-M61))</f>
-        <v>2.6715686274509793</v>
-      </c>
-      <c r="N67" s="21"/>
-      <c r="O67" s="21"/>
-      <c r="P67" s="21"/>
+      <c r="M67" s="20">
+        <f>((ABS(M66-M61)/ABS(L61-L66))*(M66-M61))</f>
+        <v>0.76454783761855882</v>
+      </c>
+      <c r="N67" t="s">
+        <v>227</v>
+      </c>
+      <c r="O67" s="19">
+        <f t="shared" si="0"/>
+        <v>-11.5</v>
+      </c>
+      <c r="P67" s="19">
+        <f t="shared" si="0"/>
+        <v>-0.76454783761855882</v>
+      </c>
     </row>
     <row r="68" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B68" t="str">
@@ -3660,17 +5857,25 @@
       <c r="K68" t="s">
         <v>222</v>
       </c>
-      <c r="L68" s="21">
+      <c r="L68" s="19">
         <f>(E5/6)*((L59-L62)/SQRT((M59-M62)^2 + (L59-L62)^2))+L62</f>
         <v>17.280254650490317</v>
       </c>
-      <c r="M68" s="21">
+      <c r="M68" s="19">
         <f>(E5/6)*((M59-M62)/SQRT((M59-M62)^2 + (L61-L62)^2))+M62</f>
         <v>2.5397977258648643</v>
       </c>
-      <c r="N68" s="21"/>
-      <c r="O68" s="21"/>
-      <c r="P68" s="21"/>
+      <c r="N68" t="s">
+        <v>222</v>
+      </c>
+      <c r="O68" s="19">
+        <f t="shared" si="0"/>
+        <v>-17.280254650490317</v>
+      </c>
+      <c r="P68" s="19">
+        <f t="shared" si="0"/>
+        <v>-2.5397977258648643</v>
+      </c>
     </row>
     <row r="69" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
@@ -3712,7 +5917,7 @@
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" s="19"/>
+      <c r="B5" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>